<commit_message>
Commit After Applying Retry mechanism in AdminUsersTest
</commit_message>
<xml_diff>
--- a/demoproject/src/test/resources/Testdatafile.xlsx
+++ b/demoproject/src/test/resources/Testdatafile.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
@@ -52,10 +52,10 @@
     <t>New Offer Alert!Don't miss out!Flash sale ends soon.</t>
   </si>
   <si>
-    <t>abc</t>
+    <t>Louis.Antoine.Pierre</t>
   </si>
   <si>
-    <t>abc@321</t>
+    <t>Louisap@123</t>
   </si>
 </sst>
 </file>
@@ -79,15 +79,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -539,12 +539,12 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -669,9 +669,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,6 +732,13 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1081,13 +1089,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="9.77777777777778" customWidth="1"/>
-    <col min="2" max="2" width="10.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="25.1111111111111" customWidth="1"/>
+    <col min="2" max="2" width="15.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1107,11 +1115,11 @@
       </c>
     </row>
     <row r="3" spans="2:2">
-      <c r="B3" s="1"/>
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="abc@321" tooltip="mailto:abc@321"/>
+    <hyperlink ref="B2" r:id="rId1" display="Louisap@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>